<commit_message>
Thermal safety margin code, figures, and analysis. uploading previous manuscript documents as well. Updated stat model output excel file.
</commit_message>
<xml_diff>
--- a/model_outputs.xlsx
+++ b/model_outputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\freezing_tolerance\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\freezing_tolerance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2A1CCE-76C5-4E20-A11B-957988782A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C2FDDB-BE8B-47B7-B016-269E7B6899F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="240" windowWidth="26340" windowHeight="18240" activeTab="2" xr2:uid="{A0FB6B5F-D5CF-4732-8622-D592A94C8237}"/>
+    <workbookView xWindow="1110" yWindow="285" windowWidth="21270" windowHeight="20070" activeTab="2" xr2:uid="{A0FB6B5F-D5CF-4732-8622-D592A94C8237}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenology" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="109">
   <si>
     <t>Estimate</t>
   </si>
@@ -326,13 +326,52 @@
   </si>
   <si>
     <t>Liriodendron tulipifera - Fagus grandifolia == 0</t>
+  </si>
+  <si>
+    <t>Comparing thermal safety margins for just 2022/2023</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>odel selec</t>
+  </si>
+  <si>
+    <t>tion tab</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>jln_dat</t>
+  </si>
+  <si>
+    <t>Coefficients:</t>
+  </si>
+  <si>
+    <t>julian_date</t>
+  </si>
+  <si>
+    <t>Tukey HSD on species</t>
+  </si>
+  <si>
+    <t>Comparing thermal safety margins against lowest temp since 1980</t>
+  </si>
+  <si>
+    <t>Std.</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +384,23 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -379,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -392,6 +448,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB59AB3-85AB-4C53-94B5-4463C9C281E8}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +803,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -996,818 +1058,1135 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17">
+        <v>27.96</v>
+      </c>
+      <c r="D17">
+        <v>19.59</v>
+      </c>
+      <c r="E17">
+        <v>1.427</v>
+      </c>
+      <c r="F17">
+        <v>0.32668000000000003</v>
+      </c>
+    </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18">
+        <v>-33.5</v>
+      </c>
+      <c r="D18">
+        <v>19.59</v>
+      </c>
+      <c r="E18">
+        <v>-1.71</v>
+      </c>
+      <c r="F18">
+        <v>0.20118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19">
+        <v>-61.46</v>
+      </c>
+      <c r="D19">
+        <v>19.59</v>
+      </c>
+      <c r="E19">
+        <v>-3.1379999999999999</v>
+      </c>
+      <c r="F19">
+        <v>4.8500000000000001E-3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E24" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>-123546.82</v>
-      </c>
-      <c r="C20">
-        <v>33824.43</v>
-      </c>
-      <c r="D20">
-        <v>-3.653</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1.15E-3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>61.31</v>
-      </c>
-      <c r="C21">
-        <v>16.72</v>
-      </c>
-      <c r="D21">
-        <v>3.6659999999999999</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1.1100000000000001E-3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>26.34</v>
-      </c>
-      <c r="C22">
-        <v>20.48</v>
-      </c>
-      <c r="D22">
-        <v>1.286</v>
-      </c>
-      <c r="E22">
-        <v>0.20979999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>-37.96</v>
-      </c>
-      <c r="C23">
-        <v>20.48</v>
-      </c>
-      <c r="D23">
-        <v>-1.853</v>
-      </c>
-      <c r="E23">
-        <v>7.5200000000000003E-2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>-123546.82</v>
+      </c>
+      <c r="C25">
+        <v>33824.43</v>
+      </c>
+      <c r="D25">
+        <v>-3.653</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.15E-3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>61.31</v>
+      </c>
+      <c r="C26">
+        <v>16.72</v>
+      </c>
+      <c r="D26">
+        <v>3.6659999999999999</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1.1100000000000001E-3</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>26.34</v>
       </c>
       <c r="C27">
-        <v>-15.4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>28</v>
+        <v>20.48</v>
+      </c>
+      <c r="D27">
+        <v>1.286</v>
       </c>
       <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>-86.286000000000001</v>
-      </c>
-      <c r="G27">
-        <v>191.7</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0.71099999999999997</v>
+        <v>0.20979999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="4">
-        <v>-14.87</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4">
-        <v>5</v>
-      </c>
-      <c r="F28" s="4">
-        <v>-90.533000000000001</v>
-      </c>
-      <c r="G28" s="4">
-        <v>193.6</v>
-      </c>
-      <c r="H28" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0.27400000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29">
-        <v>-14.87</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29">
-        <v>-96.263000000000005</v>
-      </c>
-      <c r="G29">
-        <v>199.4</v>
-      </c>
-      <c r="H29">
-        <v>7.79</v>
-      </c>
-      <c r="I29">
-        <v>1.4E-2</v>
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>-37.96</v>
+      </c>
+      <c r="C28">
+        <v>20.48</v>
+      </c>
+      <c r="D28">
+        <v>-1.853</v>
+      </c>
+      <c r="E28">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30">
-        <v>-110.25</v>
-      </c>
-      <c r="G30">
-        <v>224.9</v>
-      </c>
-      <c r="H30">
-        <v>33.28</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>40</v>
+      <c r="A31" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31">
-        <v>4</v>
-      </c>
-      <c r="F31">
-        <v>-108.248</v>
-      </c>
-      <c r="G31">
-        <v>226.1</v>
-      </c>
-      <c r="H31">
-        <v>34.43</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>-15.4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>-86.286000000000001</v>
+      </c>
+      <c r="G32">
+        <v>191.7</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0.71099999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>41</v>
+      <c r="A33" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-14.87</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4">
+        <v>-90.533000000000001</v>
+      </c>
+      <c r="G33" s="4">
+        <v>193.6</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.27400000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>-14.87</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>-96.263000000000005</v>
+      </c>
+      <c r="G34">
+        <v>199.4</v>
+      </c>
+      <c r="H34">
+        <v>7.79</v>
+      </c>
+      <c r="I34">
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>-110.25</v>
+      </c>
+      <c r="G35">
+        <v>224.9</v>
+      </c>
+      <c r="H35">
+        <v>33.28</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="4">
-        <v>58.27</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="4">
-        <v>7</v>
-      </c>
-      <c r="F36" s="4">
-        <v>-150.03899999999999</v>
-      </c>
-      <c r="G36" s="4">
-        <v>319.2</v>
-      </c>
-      <c r="H36" s="4">
-        <v>0</v>
-      </c>
-      <c r="I36" s="4">
-        <v>0.84399999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37">
-        <v>61.31</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="F37">
-        <v>-155.15100000000001</v>
-      </c>
-      <c r="G37">
-        <v>322.8</v>
-      </c>
-      <c r="H37">
-        <v>3.63</v>
-      </c>
-      <c r="I37">
-        <v>0.13700000000000001</v>
+      <c r="A36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>-108.248</v>
+      </c>
+      <c r="G36">
+        <v>226.1</v>
+      </c>
+      <c r="H36">
+        <v>34.43</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38">
-        <v>61.31</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-      <c r="F38">
-        <v>-160.017</v>
-      </c>
-      <c r="G38">
-        <v>327</v>
-      </c>
-      <c r="H38">
-        <v>7.79</v>
-      </c>
-      <c r="I38">
-        <v>1.7000000000000001E-2</v>
+      <c r="A38" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" t="s">
-        <v>28</v>
+        <v>92</v>
+      </c>
+      <c r="B39">
+        <v>3.2</v>
+      </c>
+      <c r="D39">
+        <v>2.3769999999999998</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>1.3460000000000001</v>
       </c>
       <c r="F39">
-        <v>-161.40100000000001</v>
-      </c>
-      <c r="G39">
-        <v>332.4</v>
-      </c>
-      <c r="H39">
-        <v>13.23</v>
-      </c>
-      <c r="I39">
-        <v>1E-3</v>
+        <v>0.36942999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>46</v>
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40">
+        <v>-5</v>
+      </c>
+      <c r="D40">
+        <v>2.3769999999999998</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>-2.1040000000000001</v>
       </c>
       <c r="F40">
-        <v>-164.779</v>
-      </c>
-      <c r="G40">
-        <v>334</v>
-      </c>
-      <c r="H40">
-        <v>14.83</v>
-      </c>
-      <c r="I40">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>3</v>
+        <v>8.9020000000000002E-2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="D41">
+        <v>2.3769999999999998</v>
+      </c>
+      <c r="E41">
+        <v>-3.45</v>
+      </c>
+      <c r="F41">
+        <v>1.6299999999999999E-3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43">
-        <v>-117396.32</v>
-      </c>
-      <c r="C43">
-        <v>51425.09</v>
-      </c>
-      <c r="D43">
-        <v>-2.2829999999999999</v>
-      </c>
-      <c r="E43">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="F43" t="s">
-        <v>47</v>
+      <c r="A43" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44">
-        <v>58.27</v>
-      </c>
-      <c r="C44">
-        <v>25.43</v>
-      </c>
-      <c r="D44">
-        <v>2.2919999999999998</v>
-      </c>
-      <c r="E44">
-        <v>3.1E-2</v>
-      </c>
-      <c r="F44" t="s">
-        <v>47</v>
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="4">
+        <v>58.27</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="4">
         <v>7</v>
       </c>
-      <c r="B45">
-        <v>104188.13</v>
-      </c>
-      <c r="C45">
-        <v>72726.06</v>
-      </c>
-      <c r="D45">
-        <v>1.4330000000000001</v>
-      </c>
-      <c r="E45">
-        <v>0.16489999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46">
-        <v>-122651.27</v>
-      </c>
-      <c r="C46">
-        <v>72726.06</v>
-      </c>
-      <c r="D46">
-        <v>-1.6859999999999999</v>
-      </c>
-      <c r="E46">
-        <v>0.1047</v>
+      <c r="F46" s="4">
+        <v>-150.03899999999999</v>
+      </c>
+      <c r="G46" s="4">
+        <v>319.2</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0.84399999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47">
-        <v>-51.5</v>
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
       </c>
       <c r="C47">
-        <v>35.96</v>
-      </c>
-      <c r="D47">
-        <v>-1.4319999999999999</v>
+        <v>61.31</v>
       </c>
       <c r="E47">
-        <v>0.16500000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>-155.15100000000001</v>
+      </c>
+      <c r="G47">
+        <v>322.8</v>
+      </c>
+      <c r="H47">
+        <v>3.63</v>
+      </c>
+      <c r="I47">
+        <v>0.13700000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48">
-        <v>60.62</v>
+      <c r="A48" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C48">
-        <v>35.96</v>
-      </c>
-      <c r="D48">
-        <v>1.6859999999999999</v>
+        <v>61.31</v>
       </c>
       <c r="E48">
-        <v>0.1048</v>
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>-160.017</v>
+      </c>
+      <c r="G48">
+        <v>327</v>
+      </c>
+      <c r="H48">
+        <v>7.79</v>
+      </c>
+      <c r="I48">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>-161.40100000000001</v>
+      </c>
+      <c r="G49">
+        <v>332.4</v>
+      </c>
+      <c r="H49">
+        <v>13.23</v>
+      </c>
+      <c r="I49">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" t="s">
-        <v>50</v>
+      <c r="A50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>-164.779</v>
+      </c>
+      <c r="G50">
+        <v>334</v>
+      </c>
+      <c r="H50">
+        <v>14.83</v>
+      </c>
+      <c r="I50">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>18</v>
+      <c r="A52" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" t="s">
-        <v>25</v>
-      </c>
-      <c r="I52" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C53" s="4">
-        <v>-17</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4">
-        <v>5</v>
-      </c>
-      <c r="F53" s="4">
-        <v>-103.782</v>
-      </c>
-      <c r="G53" s="4">
-        <v>220.1</v>
-      </c>
-      <c r="H53" s="4">
-        <v>0</v>
-      </c>
-      <c r="I53" s="4">
-        <v>0.64700000000000002</v>
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>-117396.32</v>
+      </c>
+      <c r="C53">
+        <v>51425.09</v>
+      </c>
+      <c r="D53">
+        <v>-2.2829999999999999</v>
+      </c>
+      <c r="E53">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>58.27</v>
       </c>
       <c r="C54">
-        <v>-19.399999999999999</v>
-      </c>
-      <c r="D54" t="s">
-        <v>28</v>
+        <v>25.43</v>
+      </c>
+      <c r="D54">
+        <v>2.2919999999999998</v>
       </c>
       <c r="E54">
-        <v>7</v>
-      </c>
-      <c r="F54">
-        <v>-101.2</v>
-      </c>
-      <c r="G54">
-        <v>221.5</v>
-      </c>
-      <c r="H54">
-        <v>1.43</v>
-      </c>
-      <c r="I54">
-        <v>0.317</v>
+        <v>3.1E-2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <v>104188.13</v>
       </c>
       <c r="C55">
-        <v>-17</v>
+        <v>72726.06</v>
+      </c>
+      <c r="D55">
+        <v>1.4330000000000001</v>
       </c>
       <c r="E55">
-        <v>3</v>
-      </c>
-      <c r="F55">
-        <v>-109.473</v>
-      </c>
-      <c r="G55">
-        <v>225.9</v>
-      </c>
-      <c r="H55">
-        <v>5.81</v>
-      </c>
-      <c r="I55">
-        <v>3.5999999999999997E-2</v>
+        <v>0.16489999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="B56">
+        <v>-122651.27</v>
+      </c>
+      <c r="C56">
+        <v>72726.06</v>
+      </c>
+      <c r="D56">
+        <v>-1.6859999999999999</v>
       </c>
       <c r="E56">
-        <v>4</v>
-      </c>
-      <c r="F56">
-        <v>-115.748</v>
-      </c>
-      <c r="G56">
-        <v>241.1</v>
-      </c>
-      <c r="H56">
-        <v>21.03</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
+        <v>0.1047</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>55</v>
+      <c r="A57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>-51.5</v>
+      </c>
+      <c r="C57">
+        <v>35.96</v>
+      </c>
+      <c r="D57">
+        <v>-1.4319999999999999</v>
       </c>
       <c r="E57">
-        <v>2</v>
-      </c>
-      <c r="F57">
-        <v>-118.58</v>
-      </c>
-      <c r="G57">
-        <v>241.6</v>
-      </c>
-      <c r="H57">
-        <v>21.54</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58">
+        <v>60.62</v>
+      </c>
+      <c r="C58">
+        <v>35.96</v>
+      </c>
+      <c r="D58">
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="E58">
+        <v>0.1048</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+      <c r="A60" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="B60" t="s">
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D60" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="E60" t="s">
-        <v>3</v>
+        <v>78</v>
+      </c>
+      <c r="F60" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="B61">
-        <v>34485.599999999999</v>
-      </c>
-      <c r="C61">
-        <v>6103.6940000000004</v>
+        <v>104188</v>
       </c>
       <c r="D61">
-        <v>5.65</v>
-      </c>
-      <c r="E61" s="3">
-        <v>6.1E-6</v>
-      </c>
-      <c r="F61" t="s">
-        <v>5</v>
+        <v>72726</v>
+      </c>
+      <c r="E61">
+        <v>1.4330000000000001</v>
+      </c>
+      <c r="F61">
+        <v>0.3241</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62">
+        <v>-122651</v>
+      </c>
+      <c r="D62">
+        <v>72726</v>
+      </c>
+      <c r="E62">
+        <v>-1.6859999999999999</v>
+      </c>
+      <c r="F62">
+        <v>0.21037</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63">
+        <v>-226839</v>
+      </c>
+      <c r="D63">
+        <v>72726</v>
+      </c>
+      <c r="E63">
+        <v>-3.1190000000000002</v>
+      </c>
+      <c r="F63">
+        <v>5.2199999999999998E-3</v>
+      </c>
+      <c r="G63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="4">
+        <v>-17</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4">
+        <v>5</v>
+      </c>
+      <c r="F69" s="4">
+        <v>-103.782</v>
+      </c>
+      <c r="G69" s="4">
+        <v>220.1</v>
+      </c>
+      <c r="H69" s="4">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70">
+        <v>-19.399999999999999</v>
+      </c>
+      <c r="D70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70">
+        <v>7</v>
+      </c>
+      <c r="F70">
+        <v>-101.2</v>
+      </c>
+      <c r="G70">
+        <v>221.5</v>
+      </c>
+      <c r="H70">
+        <v>1.43</v>
+      </c>
+      <c r="I70">
+        <v>0.317</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71">
+        <v>-17</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>-109.473</v>
+      </c>
+      <c r="G71">
+        <v>225.9</v>
+      </c>
+      <c r="H71">
+        <v>5.81</v>
+      </c>
+      <c r="I71">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B72" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+      <c r="F72">
+        <v>-115.748</v>
+      </c>
+      <c r="G72">
+        <v>241.1</v>
+      </c>
+      <c r="H72">
+        <v>21.03</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>-118.58</v>
+      </c>
+      <c r="G73">
+        <v>241.6</v>
+      </c>
+      <c r="H73">
+        <v>21.54</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77">
+        <v>34485.599999999999</v>
+      </c>
+      <c r="C77">
+        <v>6103.6940000000004</v>
+      </c>
+      <c r="D77">
+        <v>5.65</v>
+      </c>
+      <c r="E77" s="3">
+        <v>6.1E-6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B62">
+      <c r="B78">
         <v>-17</v>
       </c>
-      <c r="C62">
+      <c r="C78">
         <v>3.0179999999999998</v>
       </c>
-      <c r="D62">
+      <c r="D78">
         <v>-5.633</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E78" s="3">
         <v>6.3799999999999999E-6</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F78" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B63">
+      <c r="B79">
         <v>6.2</v>
       </c>
-      <c r="C63">
+      <c r="C79">
         <v>3.6960000000000002</v>
       </c>
-      <c r="D63">
+      <c r="D79">
         <v>1.677</v>
       </c>
-      <c r="E63">
+      <c r="E79">
         <v>0.10539999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B64">
+      <c r="B80">
         <v>-6.6</v>
       </c>
-      <c r="C64">
+      <c r="C80">
         <v>3.6960000000000002</v>
       </c>
-      <c r="D64">
+      <c r="D80">
         <v>-1.786</v>
       </c>
-      <c r="E64">
+      <c r="E80">
         <v>8.5800000000000001E-2</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F80" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" t="s">
+        <v>107</v>
+      </c>
+      <c r="E82" t="s">
+        <v>78</v>
+      </c>
+      <c r="F82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83">
+        <v>6.2</v>
+      </c>
+      <c r="D83">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="E83">
+        <v>1.677</v>
+      </c>
+      <c r="F83">
+        <v>0.21387</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84">
+        <v>-6.6</v>
+      </c>
+      <c r="D84">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="E84">
+        <v>-1.786</v>
+      </c>
+      <c r="F84">
+        <v>0.17438000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85">
+        <v>-12.8</v>
+      </c>
+      <c r="D85">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="E85">
+        <v>-3.4630000000000001</v>
+      </c>
+      <c r="F85">
+        <v>1.57E-3</v>
+      </c>
+      <c r="G85" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1818,7 +2197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E3CB38-395B-4398-A84F-647C15042239}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
@@ -2939,12 +3318,955 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AA81AB-ED88-48D5-A624-55AC38D9E4FB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>-5400</v>
+      </c>
+      <c r="C5" s="4">
+        <v>9.2069999999999999E-2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.673</v>
+      </c>
+      <c r="F5" s="4">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-626.78700000000003</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1266</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.88700000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>-5399</v>
+      </c>
+      <c r="C6">
+        <v>9.2069999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.673</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>-630.95899999999995</v>
+      </c>
+      <c r="H6">
+        <v>1270.0999999999999</v>
+      </c>
+      <c r="I6">
+        <v>4.13</v>
+      </c>
+      <c r="J6">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>6.9880000000000004</v>
+      </c>
+      <c r="C7">
+        <v>8.8220000000000007E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>-636.25</v>
+      </c>
+      <c r="H7">
+        <v>1282.8</v>
+      </c>
+      <c r="I7">
+        <v>16.809999999999999</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>8.2010000000000005</v>
+      </c>
+      <c r="C8">
+        <v>8.8220000000000007E-2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>-640.07899999999995</v>
+      </c>
+      <c r="H8">
+        <v>1286.3</v>
+      </c>
+      <c r="I8">
+        <v>20.29</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>-4710</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>-653.18399999999997</v>
+      </c>
+      <c r="H9">
+        <v>1316.7</v>
+      </c>
+      <c r="I9">
+        <v>50.68</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>-4709</v>
+      </c>
+      <c r="E10">
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>-656.46500000000003</v>
+      </c>
+      <c r="H10">
+        <v>1319</v>
+      </c>
+      <c r="I10">
+        <v>53.07</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>14.31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>-658.97</v>
+      </c>
+      <c r="H11">
+        <v>1326.1</v>
+      </c>
+      <c r="I11">
+        <v>60.15</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>15.52</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>-662.08299999999997</v>
+      </c>
+      <c r="H12">
+        <v>1328.2</v>
+      </c>
+      <c r="I12">
+        <v>62.25</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <v>-5400</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1230</v>
+      </c>
+      <c r="D16">
+        <v>-4.3899999999999997</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.7900000000000001E-5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="3">
+        <v>9.2069999999999999E-2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.205E-2</v>
+      </c>
+      <c r="D17">
+        <v>7.6429999999999998</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7.34E-13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2.673</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.60819999999999996</v>
+      </c>
+      <c r="D18">
+        <v>4.3959999999999999</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1.7499999999999998E-5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.7429</v>
+      </c>
+      <c r="D19">
+        <v>2.7280000000000002</v>
+      </c>
+      <c r="E19">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.7429</v>
+      </c>
+      <c r="D20">
+        <v>2.17</v>
+      </c>
+      <c r="E20">
+        <v>3.1099999999999999E-2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.7429</v>
+      </c>
+      <c r="D23">
+        <v>2.7280000000000002</v>
+      </c>
+      <c r="E23">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24">
+        <v>1.6123000000000001</v>
+      </c>
+      <c r="C24">
+        <v>0.7429</v>
+      </c>
+      <c r="D24">
+        <v>2.17</v>
+      </c>
+      <c r="E24">
+        <v>7.6399999999999996E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25">
+        <v>-0.41470000000000001</v>
+      </c>
+      <c r="C25">
+        <v>0.7429</v>
+      </c>
+      <c r="D25">
+        <v>-0.55800000000000005</v>
+      </c>
+      <c r="E25">
+        <v>0.84230000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>8</v>
+      </c>
+      <c r="B31" s="4">
+        <v>-6310</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.10489999999999999</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3.12</v>
+      </c>
+      <c r="F31" s="4">
+        <v>6</v>
+      </c>
+      <c r="G31" s="4">
+        <v>-608.86599999999999</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1230.0999999999999</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>-6309</v>
+      </c>
+      <c r="C32">
+        <v>0.10489999999999999</v>
+      </c>
+      <c r="E32">
+        <v>3.12</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>-613.77499999999998</v>
+      </c>
+      <c r="H32">
+        <v>1235.7</v>
+      </c>
+      <c r="I32">
+        <v>5.6</v>
+      </c>
+      <c r="J32">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>1.097</v>
+      </c>
+      <c r="C33">
+        <v>0.1004</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>-623.70399999999995</v>
+      </c>
+      <c r="H33">
+        <v>1257.7</v>
+      </c>
+      <c r="I33">
+        <v>27.56</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>2.31</v>
+      </c>
+      <c r="C34">
+        <v>0.1004</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>-627.99400000000003</v>
+      </c>
+      <c r="H34">
+        <v>1262.0999999999999</v>
+      </c>
+      <c r="I34">
+        <v>31.97</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>-5524</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35">
+        <v>2.7360000000000002</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>-647.03800000000001</v>
+      </c>
+      <c r="H35">
+        <v>1304.4000000000001</v>
+      </c>
+      <c r="I35">
+        <v>74.23</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>-5523</v>
+      </c>
+      <c r="E36">
+        <v>2.7360000000000002</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>-650.50800000000004</v>
+      </c>
+      <c r="H36">
+        <v>1307.0999999999999</v>
+      </c>
+      <c r="I36">
+        <v>77</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>9.4269999999999996</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>-655.34299999999996</v>
+      </c>
+      <c r="H37">
+        <v>1318.9</v>
+      </c>
+      <c r="I37">
+        <v>88.74</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>10.64</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>-658.56</v>
+      </c>
+      <c r="H38">
+        <v>1321.2</v>
+      </c>
+      <c r="I38">
+        <v>91.04</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3">
+        <v>-6310</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1132</v>
+      </c>
+      <c r="D41">
+        <v>-5.5730000000000004</v>
+      </c>
+      <c r="E41" s="3">
+        <v>7.5800000000000004E-8</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.10489999999999999</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1.1089999999999999E-2</v>
+      </c>
+      <c r="D42">
+        <v>9.4580000000000002</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.55979999999999996</v>
+      </c>
+      <c r="D43">
+        <v>5.5739999999999998</v>
+      </c>
+      <c r="E43" s="3">
+        <v>7.54E-8</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.68369999999999997</v>
+      </c>
+      <c r="D44">
+        <v>2.9649999999999999</v>
+      </c>
+      <c r="E44">
+        <v>3.3800000000000002E-3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.68369999999999997</v>
+      </c>
+      <c r="D45">
+        <v>2.3580000000000001</v>
+      </c>
+      <c r="E45">
+        <v>1.9290000000000002E-2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="C48">
+        <v>0.68369999999999997</v>
+      </c>
+      <c r="D48">
+        <v>2.9649999999999999</v>
+      </c>
+      <c r="E48">
+        <v>8.43E-3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49">
+        <v>1.6123000000000001</v>
+      </c>
+      <c r="C49">
+        <v>0.68369999999999997</v>
+      </c>
+      <c r="D49">
+        <v>2.3580000000000001</v>
+      </c>
+      <c r="E49">
+        <v>4.8149999999999998E-2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50">
+        <v>-0.41470000000000001</v>
+      </c>
+      <c r="C50">
+        <v>0.68369999999999997</v>
+      </c>
+      <c r="D50">
+        <v>-0.60599999999999998</v>
+      </c>
+      <c r="E50">
+        <v>0.81659000000000004</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>